<commit_message>
Regenerate all penyata to follow new data and format
</commit_message>
<xml_diff>
--- a/penyata-akhir-2023/form1/1AMANAH-2023.xlsx
+++ b/penyata-akhir-2023/form1/1AMANAH-2023.xlsx
@@ -3,9 +3,6 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" firstSheet="0" activeTab="0"/>
-  </bookViews>
   <sheets>
     <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
   </sheets>
@@ -14,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>UNIT PEMBANGUNAN</t>
   </si>
@@ -58,16 +55,16 @@
     <t>Penandaan Fail</t>
   </si>
   <si>
-    <t>Kali Pertama</t>
-  </si>
-  <si>
-    <t>Kali Kedua</t>
-  </si>
-  <si>
-    <t>Kali Ketiga</t>
-  </si>
-  <si>
-    <t>Kali Keempat</t>
+    <t>Semakan Kali Pertama</t>
+  </si>
+  <si>
+    <t>Semakan Kali Kedua</t>
+  </si>
+  <si>
+    <t>Semakan Kali Ketiga</t>
+  </si>
+  <si>
+    <t>Semakan Kali Keempat</t>
   </si>
   <si>
     <t>Laporan Atas Talian (Google Form)</t>
@@ -79,16 +76,25 @@
     <t>Penyertaan Pertandingan</t>
   </si>
   <si>
-    <t>BOUQUET KREATIF</t>
-  </si>
-  <si>
-    <t>KAD RAYA UNTUK GURUKU</t>
-  </si>
-  <si>
-    <t>RIANG RIA KUIH RAYA</t>
-  </si>
-  <si>
-    <t>CREATIVE COLLAGE</t>
+    <t>Bouquet Kreatif</t>
+  </si>
+  <si>
+    <t>Kad Raya Untuk Guruku</t>
+  </si>
+  <si>
+    <t>Riang Ria Kuih Raya</t>
+  </si>
+  <si>
+    <t>Creative Collage</t>
+  </si>
+  <si>
+    <t>Lompat Getah</t>
+  </si>
+  <si>
+    <t>Theme Party</t>
+  </si>
+  <si>
+    <t>Hari Koperasi</t>
   </si>
   <si>
     <t/>
@@ -116,38 +122,28 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <charset val="1"/>
       <color rgb="FF000000"/>
       <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
-      <charset val="1"/>
       <color rgb="FF000000"/>
       <sz val="10"/>
       <name val="Merriweather"/>
     </font>
     <font>
-      <charset val="1"/>
       <color rgb="FF000000"/>
       <sz val="25"/>
       <name val="Impact"/>
     </font>
     <font>
-      <charset val="1"/>
       <color rgb="FFFF0000"/>
       <sz val="10"/>
       <name val="Impact"/>
     </font>
-    <font>
-      <charset val="1"/>
-      <color rgb="FF000000"/>
-      <sz val="9"/>
-      <name val="Arial"/>
-    </font>
+    <font/>
     <font>
       <b/>
-      <charset val="1"/>
       <color rgb="FF000000"/>
       <sz val="10"/>
       <name val="Arial"/>
@@ -155,20 +151,17 @@
     <font>
       <b/>
       <i/>
-      <charset val="1"/>
       <color rgb="FF000000"/>
       <sz val="9"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <charset val="1"/>
       <color rgb="FF000000"/>
       <sz val="9"/>
       <name val="Arial"/>
     </font>
     <font>
-      <charset val="1"/>
       <color rgb="FF000000"/>
       <sz val="10"/>
       <name val="Cambria"/>
@@ -176,21 +169,18 @@
     <font>
       <b/>
       <i/>
-      <charset val="1"/>
       <color rgb="FF000000"/>
       <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <charset val="1"/>
       <color rgb="FF000000"/>
       <sz val="12"/>
       <name val="Arial"/>
     </font>
     <font>
       <i/>
-      <charset val="1"/>
       <color rgb="FF000000"/>
       <sz val="14"/>
       <name val="Caveat"/>
@@ -212,17 +202,17 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFE599"/>
-        <bgColor rgb="FFFFFF99"/>
+        <bgColor rgb="FFFFE599"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF666666"/>
-        <bgColor rgb="FF808080"/>
+        <bgColor rgb="FF666666"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -280,66 +270,144 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin"/>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
       <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin"/>
-      <top style="thin"/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
       <top/>
-      <bottom style="double"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -377,7 +445,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
@@ -403,82 +471,90 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="bottom" wrapText="1" shrinkToFit="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="bottom" wrapText="1" shrinkToFit="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="bottom" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -500,19 +576,14 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:oneCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>85680</xdr:colOff>
+      <xdr:colOff>152400</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>580320</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>65880</xdr:rowOff>
-    </xdr:to>
+    <xdr:ext cx="590550" cy="600075"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="1" name="Picture 1">
@@ -543,27 +614,221 @@
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+  <a:themeElements>
+    <a:clrScheme name="Sheets">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="FFFFFF"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="0000FF"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Sheets">
+      <a:majorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface="Calibri"/>
+        <a:cs typeface="Calibri"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface="Calibri"/>
+        <a:cs typeface="Calibri"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1001"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100" view="normal">
-      <selection activeCell="C37" sqref="C37"/>
-    </sheetView>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0" defaultColWidth="14.4375"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0" defaultColWidth="14.43"/>
   <cols>
-    <col min="1" max="1" width="4.85" customWidth="1"/>
+    <col min="1" max="1" width="4.86" customWidth="1"/>
     <col min="2" max="2" width="12.57" customWidth="1"/>
     <col min="3" max="3" width="33" customWidth="1"/>
     <col min="4" max="5" width="12.57" customWidth="1"/>
     <col min="6" max="6" width="13.43" customWidth="1"/>
     <col min="7" max="7" width="5.57" customWidth="1"/>
-    <col min="8" max="26" width="12.57" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -591,18 +856,20 @@
     </row>
     <row r="4" ht="14.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
-      <c r="C4" s="7"/>
-      <c r="E4" s="8" t="s">
+      <c r="C4"/>
+      <c r="D4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="6"/>
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4" s="9"/>
     </row>
     <row r="5" ht="15.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
+      <c r="C5"/>
       <c r="G5" s="6"/>
     </row>
     <row r="6" ht="15.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -614,26 +881,26 @@
       <c r="B7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="12"/>
       <c r="G7" s="6"/>
     </row>
     <row r="8" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
+      <c r="C8"/>
+      <c r="D8" s="14"/>
       <c r="G8" s="6"/>
     </row>
     <row r="9" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="17"/>
       <c r="G9" s="6"/>
     </row>
     <row r="10" ht="15.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -646,124 +913,125 @@
     </row>
     <row r="12" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
       <c r="G12" s="6"/>
     </row>
     <row r="13" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15" t="s">
+      <c r="C13" s="20"/>
+      <c r="D13" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="22" t="s">
         <v>11</v>
       </c>
       <c r="G13" s="6"/>
     </row>
     <row r="14" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="18">
+      <c r="C14" s="20"/>
+      <c r="D14" s="24">
         <v>500</v>
       </c>
-      <c r="E14" s="18"/>
-      <c r="F14" s="19">
+      <c r="E14" s="24"/>
+      <c r="F14" s="25">
         <v>1000</v>
       </c>
       <c r="G14" s="6"/>
     </row>
     <row r="15" ht="15.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="24"/>
       <c r="G15" s="6"/>
     </row>
     <row r="16" ht="15.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="21" t="s">
+      <c r="B16" s="23"/>
+      <c r="C16" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="22">
+      <c r="D16" s="29">
         <v>2850</v>
       </c>
-      <c r="E16" s="23">
+      <c r="E16" s="30">
         <v>300</v>
       </c>
-      <c r="F16" s="18"/>
+      <c r="F16" s="24"/>
       <c r="G16" s="6"/>
     </row>
     <row r="17" ht="15.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="21" t="s">
+      <c r="B17" s="23"/>
+      <c r="C17" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="22">
+      <c r="D17" s="29">
         <v>3000</v>
       </c>
-      <c r="E17" s="18">
+      <c r="E17" s="24">
         <v>1700</v>
       </c>
-      <c r="F17" s="18"/>
+      <c r="F17" s="24"/>
       <c r="G17" s="6"/>
     </row>
     <row r="18" ht="15.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="21" t="s">
+      <c r="B18" s="23"/>
+      <c r="C18" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="22">
-        <v>0</v>
-      </c>
-      <c r="E18" s="18">
-        <v>0</v>
-      </c>
-      <c r="F18" s="18"/>
+      <c r="D18" s="29">
+        <v>3085</v>
+      </c>
+      <c r="E18" s="24">
+        <v>1750</v>
+      </c>
+      <c r="F18" s="24"/>
       <c r="G18" s="6"/>
     </row>
     <row r="19" ht="15.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="21" t="s">
+      <c r="B19" s="23"/>
+      <c r="C19" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="22">
-        <v>0</v>
-      </c>
-      <c r="E19" s="18">
-        <v>0</v>
-      </c>
-      <c r="F19" s="18"/>
+      <c r="D19" s="29">
+        <v>0</v>
+      </c>
+      <c r="E19" s="24">
+        <v>0</v>
+      </c>
+      <c r="F19" s="24"/>
       <c r="G19" s="6"/>
     </row>
     <row r="20" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="25">
+      <c r="B20" s="31"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="32">
         <f>D16-E16+D17-E17+D18-E18+D19-E19+F14</f>
         <v>1000</v>
       </c>
@@ -771,82 +1039,82 @@
     </row>
     <row r="21" ht="15.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="24"/>
       <c r="G21" s="6"/>
     </row>
     <row r="22" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="21" t="s">
+      <c r="B22" s="23"/>
+      <c r="C22" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="22">
-        <v>0</v>
-      </c>
-      <c r="E22" s="18">
-        <v>0</v>
-      </c>
-      <c r="F22" s="18"/>
+      <c r="D22" s="29">
+        <v>0</v>
+      </c>
+      <c r="E22" s="24">
+        <v>0</v>
+      </c>
+      <c r="F22" s="24"/>
       <c r="G22" s="6"/>
     </row>
     <row r="23" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="21" t="s">
+      <c r="B23" s="23"/>
+      <c r="C23" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="22">
-        <v>0</v>
-      </c>
-      <c r="E23" s="18">
-        <v>0</v>
-      </c>
-      <c r="F23" s="18"/>
+      <c r="D23" s="29">
+        <v>0</v>
+      </c>
+      <c r="E23" s="24">
+        <v>0</v>
+      </c>
+      <c r="F23" s="24"/>
       <c r="G23" s="6"/>
     </row>
     <row r="24" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="21" t="s">
+      <c r="B24" s="23"/>
+      <c r="C24" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="22">
-        <v>0</v>
-      </c>
-      <c r="E24" s="18">
-        <v>0</v>
-      </c>
-      <c r="F24" s="18"/>
+      <c r="D24" s="29">
+        <v>0</v>
+      </c>
+      <c r="E24" s="24">
+        <v>0</v>
+      </c>
+      <c r="F24" s="24"/>
       <c r="G24" s="6"/>
     </row>
     <row r="25" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="21" t="s">
+      <c r="B25" s="23"/>
+      <c r="C25" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="D25" s="22">
-        <v>0</v>
-      </c>
-      <c r="E25" s="18">
-        <v>0</v>
-      </c>
-      <c r="F25" s="18"/>
+      <c r="D25" s="29">
+        <v>0</v>
+      </c>
+      <c r="E25" s="24">
+        <v>0</v>
+      </c>
+      <c r="F25" s="24"/>
       <c r="G25" s="6"/>
     </row>
     <row r="26" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="25">
+      <c r="B26" s="31"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="32">
         <f>D23-E23+D24-E24+D25-E25-E22+D22</f>
         <v>0</v>
       </c>
@@ -854,74 +1122,74 @@
     </row>
     <row r="27" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="10"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="24"/>
       <c r="G27" s="6"/>
     </row>
     <row r="28" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="27" t="s">
+      <c r="B28" s="10"/>
+      <c r="C28" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="28"/>
-      <c r="E28" s="18">
-        <v>0</v>
-      </c>
-      <c r="F28" s="18"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="24">
+        <v>0</v>
+      </c>
+      <c r="F28" s="24"/>
       <c r="G28" s="6"/>
     </row>
     <row r="29" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="21" t="s">
+      <c r="B29" s="23"/>
+      <c r="C29" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="28"/>
-      <c r="E29" s="18">
-        <v>0</v>
-      </c>
-      <c r="F29" s="18"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="24">
+        <v>1750</v>
+      </c>
+      <c r="F29" s="24"/>
       <c r="G29" s="6"/>
     </row>
     <row r="30" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="21" t="s">
+      <c r="B30" s="23"/>
+      <c r="C30" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="28"/>
-      <c r="E30" s="18">
-        <v>0</v>
-      </c>
-      <c r="F30" s="18"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="24">
+        <v>0</v>
+      </c>
+      <c r="F30" s="24"/>
       <c r="G30" s="6"/>
     </row>
     <row r="31" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="21" t="s">
+      <c r="B31" s="23"/>
+      <c r="C31" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="D31" s="28"/>
-      <c r="E31" s="18">
-        <v>0</v>
-      </c>
-      <c r="F31" s="18"/>
+      <c r="D31" s="35"/>
+      <c r="E31" s="24">
+        <v>0</v>
+      </c>
+      <c r="F31" s="24"/>
       <c r="G31" s="6"/>
     </row>
     <row r="32" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
-      <c r="B32" s="24"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="24"/>
-      <c r="F32" s="25">
+      <c r="B32" s="31"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="32">
         <f>-E28-E29-E30-E31</f>
         <v>0</v>
       </c>
@@ -929,136 +1197,142 @@
     </row>
     <row r="33" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C33" s="10"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="24"/>
       <c r="G33" s="6"/>
     </row>
     <row r="34" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="21" t="s">
+      <c r="B34" s="23"/>
+      <c r="C34" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="22">
+      <c r="D34" s="29">
         <v>500</v>
       </c>
-      <c r="E34" s="18">
-        <v>0</v>
-      </c>
-      <c r="F34" s="18"/>
+      <c r="E34" s="24">
+        <v>0</v>
+      </c>
+      <c r="F34" s="24"/>
       <c r="G34" s="6"/>
     </row>
     <row r="35" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="21" t="s">
+      <c r="B35" s="23"/>
+      <c r="C35" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="D35" s="22">
+      <c r="D35" s="29">
         <v>100</v>
       </c>
-      <c r="E35" s="18">
-        <v>0</v>
-      </c>
-      <c r="F35" s="18"/>
+      <c r="E35" s="24">
+        <v>0</v>
+      </c>
+      <c r="F35" s="24"/>
       <c r="G35" s="6"/>
     </row>
     <row r="36" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="21" t="s">
+      <c r="B36" s="23"/>
+      <c r="C36" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="D36" s="22">
+      <c r="D36" s="29">
         <v>100</v>
       </c>
-      <c r="E36" s="18">
-        <v>0</v>
-      </c>
-      <c r="F36" s="18"/>
+      <c r="E36" s="24">
+        <v>0</v>
+      </c>
+      <c r="F36" s="24"/>
       <c r="G36" s="6"/>
     </row>
     <row r="37" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="21" t="s">
+      <c r="B37" s="23"/>
+      <c r="C37" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="D37" s="22">
-        <v>0</v>
-      </c>
-      <c r="E37" s="18">
-        <v>0</v>
-      </c>
-      <c r="F37" s="18"/>
+      <c r="D37" s="29">
+        <v>0</v>
+      </c>
+      <c r="E37" s="24">
+        <v>0</v>
+      </c>
+      <c r="F37" s="24"/>
       <c r="G37" s="6"/>
     </row>
     <row r="38" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
-      <c r="B38" s="20"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="22">
-        <v>0</v>
-      </c>
-      <c r="E38" s="18">
-        <v>0</v>
-      </c>
-      <c r="F38" s="18"/>
+      <c r="B38" s="23"/>
+      <c r="C38" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="D38" s="29">
+        <v>300</v>
+      </c>
+      <c r="E38" s="24">
+        <v>0</v>
+      </c>
+      <c r="F38" s="24"/>
       <c r="G38" s="6"/>
     </row>
     <row r="39" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
-      <c r="B39" s="20"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="22">
-        <v>0</v>
-      </c>
-      <c r="E39" s="18">
-        <v>0</v>
-      </c>
-      <c r="F39" s="18"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="D39" s="29">
+        <v>100</v>
+      </c>
+      <c r="E39" s="24">
+        <v>0</v>
+      </c>
+      <c r="F39" s="24"/>
       <c r="G39" s="6"/>
     </row>
     <row r="40" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
-      <c r="B40" s="20"/>
-      <c r="C40" s="21"/>
-      <c r="D40" s="21">
-        <v>0</v>
-      </c>
-      <c r="E40" s="17">
-        <v>0</v>
-      </c>
-      <c r="F40" s="18"/>
+      <c r="B40" s="23"/>
+      <c r="C40" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="D40" s="36">
+        <v>0</v>
+      </c>
+      <c r="E40" s="27">
+        <v>0</v>
+      </c>
+      <c r="F40" s="24"/>
       <c r="G40" s="6"/>
     </row>
     <row r="41" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
-      <c r="B41" s="20"/>
-      <c r="C41" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D41" s="21">
-        <v>0</v>
-      </c>
-      <c r="E41" s="17">
-        <v>0</v>
-      </c>
-      <c r="F41" s="18"/>
+      <c r="B41" s="23"/>
+      <c r="C41" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="D41" s="36">
+        <v>0</v>
+      </c>
+      <c r="E41" s="27">
+        <v>0</v>
+      </c>
+      <c r="F41" s="24"/>
       <c r="G41" s="6"/>
     </row>
     <row r="42" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
-      <c r="B42" s="24"/>
-      <c r="C42" s="24"/>
-      <c r="D42" s="24"/>
-      <c r="E42" s="24"/>
-      <c r="F42" s="25">
+      <c r="B42" s="31"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="32">
         <f>D34-E34+D35-E35+D36-E36+D37-E37+D38-E38+D39-E39+D41-E41+D40-E40</f>
         <v>0</v>
       </c>
@@ -1066,10 +1340,13 @@
     </row>
     <row r="43" ht="15.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
-      <c r="B43" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="F43" s="30">
+      <c r="B43" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="C43"/>
+      <c r="D43"/>
+      <c r="E43"/>
+      <c r="F43" s="38">
         <f>F20+F32+F26+F42</f>
         <v>1000</v>
       </c>
@@ -1081,34 +1358,34 @@
     </row>
     <row r="45" ht="18.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
-      <c r="B45" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="C45" s="31"/>
-      <c r="D45" s="31"/>
-      <c r="E45" s="31"/>
-      <c r="F45" s="31"/>
+      <c r="B45" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C45"/>
+      <c r="D45"/>
+      <c r="E45"/>
+      <c r="F45"/>
       <c r="G45" s="6"/>
     </row>
     <row r="46" ht="18.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
-      <c r="B46" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="C46" s="31"/>
-      <c r="D46" s="31"/>
-      <c r="E46" s="31"/>
-      <c r="F46" s="31"/>
+      <c r="B46" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="C46"/>
+      <c r="D46"/>
+      <c r="E46"/>
+      <c r="F46"/>
       <c r="G46" s="6"/>
     </row>
     <row r="47" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="32"/>
-      <c r="B47" s="33"/>
-      <c r="C47" s="33"/>
-      <c r="D47" s="33"/>
-      <c r="E47" s="33"/>
-      <c r="F47" s="33"/>
-      <c r="G47" s="34"/>
+      <c r="A47" s="40"/>
+      <c r="B47" s="41"/>
+      <c r="C47" s="41"/>
+      <c r="D47" s="41"/>
+      <c r="E47" s="41"/>
+      <c r="F47" s="41"/>
+      <c r="G47" s="42"/>
     </row>
     <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2063,28 +2340,31 @@
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="19">
     <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="B5:C5"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B12:F12"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
     <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B21:E21"/>
     <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B27:E27"/>
     <mergeCell ref="B32:E32"/>
-    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B33:E33"/>
     <mergeCell ref="B42:E42"/>
+    <mergeCell ref="B43:E43"/>
     <mergeCell ref="B45:F45"/>
     <mergeCell ref="B46:F46"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" pageOrder="overThenDown" scale="100" fitToWidth="1" fitToHeight="0" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" pageOrder="overThenDown" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
:stars: Final generation for 2023
</commit_message>
<xml_diff>
--- a/penyata-akhir-2023/form1/1AMANAH-2023.xlsx
+++ b/penyata-akhir-2023/form1/1AMANAH-2023.xlsx
@@ -445,7 +445,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
@@ -508,9 +508,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -529,7 +527,6 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="bottom" wrapText="1" shrinkToFit="1" readingOrder="1"/>
     </xf>
@@ -1042,8 +1039,8 @@
       <c r="B21" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
       <c r="E21" s="20"/>
       <c r="F21" s="24"/>
       <c r="G21" s="6"/>
@@ -1088,7 +1085,7 @@
         <v>0</v>
       </c>
       <c r="E24" s="24">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F24" s="24"/>
       <c r="G24" s="6"/>
@@ -1125,8 +1122,8 @@
       <c r="B27" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
       <c r="E27" s="20"/>
       <c r="F27" s="24"/>
       <c r="G27" s="6"/>
@@ -1134,10 +1131,10 @@
     <row r="28" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="10"/>
-      <c r="C28" s="34" t="s">
+      <c r="C28" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="35"/>
+      <c r="D28" s="34"/>
       <c r="E28" s="24">
         <v>0</v>
       </c>
@@ -1150,7 +1147,7 @@
       <c r="C29" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="35"/>
+      <c r="D29" s="34"/>
       <c r="E29" s="24">
         <v>1750</v>
       </c>
@@ -1163,7 +1160,7 @@
       <c r="C30" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="35"/>
+      <c r="D30" s="34"/>
       <c r="E30" s="24">
         <v>0</v>
       </c>
@@ -1176,7 +1173,7 @@
       <c r="C31" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="D31" s="35"/>
+      <c r="D31" s="34"/>
       <c r="E31" s="24">
         <v>0</v>
       </c>
@@ -1200,8 +1197,8 @@
       <c r="B33" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C33" s="33"/>
-      <c r="D33" s="33"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
       <c r="E33" s="20"/>
       <c r="F33" s="24"/>
       <c r="G33" s="6"/>
@@ -1209,7 +1206,7 @@
     <row r="34" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="23"/>
-      <c r="C34" s="36" t="s">
+      <c r="C34" s="35" t="s">
         <v>21</v>
       </c>
       <c r="D34" s="29">
@@ -1224,7 +1221,7 @@
     <row r="35" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="23"/>
-      <c r="C35" s="36" t="s">
+      <c r="C35" s="35" t="s">
         <v>22</v>
       </c>
       <c r="D35" s="29">
@@ -1239,7 +1236,7 @@
     <row r="36" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="23"/>
-      <c r="C36" s="36" t="s">
+      <c r="C36" s="35" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="29">
@@ -1254,7 +1251,7 @@
     <row r="37" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="23"/>
-      <c r="C37" s="36" t="s">
+      <c r="C37" s="35" t="s">
         <v>24</v>
       </c>
       <c r="D37" s="29">
@@ -1269,7 +1266,7 @@
     <row r="38" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="23"/>
-      <c r="C38" s="36" t="s">
+      <c r="C38" s="35" t="s">
         <v>25</v>
       </c>
       <c r="D38" s="29">
@@ -1284,7 +1281,7 @@
     <row r="39" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="23"/>
-      <c r="C39" s="36" t="s">
+      <c r="C39" s="35" t="s">
         <v>26</v>
       </c>
       <c r="D39" s="29">
@@ -1299,10 +1296,10 @@
     <row r="40" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="23"/>
-      <c r="C40" s="36" t="s">
+      <c r="C40" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="D40" s="36">
+      <c r="D40" s="35">
         <v>0</v>
       </c>
       <c r="E40" s="27">
@@ -1314,10 +1311,10 @@
     <row r="41" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="23"/>
-      <c r="C41" s="36" t="s">
+      <c r="C41" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="D41" s="36">
+      <c r="D41" s="35">
         <v>0</v>
       </c>
       <c r="E41" s="27">
@@ -1340,13 +1337,13 @@
     </row>
     <row r="43" ht="15.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
-      <c r="B43" s="37" t="s">
+      <c r="B43" s="36" t="s">
         <v>29</v>
       </c>
       <c r="C43"/>
       <c r="D43"/>
       <c r="E43"/>
-      <c r="F43" s="38">
+      <c r="F43" s="37">
         <f>F20+F32+F26+F42</f>
         <v>1000</v>
       </c>
@@ -1358,7 +1355,7 @@
     </row>
     <row r="45" ht="18.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
-      <c r="B45" s="39" t="s">
+      <c r="B45" s="38" t="s">
         <v>30</v>
       </c>
       <c r="C45"/>
@@ -1369,7 +1366,7 @@
     </row>
     <row r="46" ht="18.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
-      <c r="B46" s="39" t="s">
+      <c r="B46" s="38" t="s">
         <v>31</v>
       </c>
       <c r="C46"/>
@@ -1379,13 +1376,13 @@
       <c r="G46" s="6"/>
     </row>
     <row r="47" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="40"/>
-      <c r="B47" s="41"/>
-      <c r="C47" s="41"/>
-      <c r="D47" s="41"/>
-      <c r="E47" s="41"/>
-      <c r="F47" s="41"/>
-      <c r="G47" s="42"/>
+      <c r="A47" s="39"/>
+      <c r="B47" s="40"/>
+      <c r="C47" s="40"/>
+      <c r="D47" s="40"/>
+      <c r="E47" s="40"/>
+      <c r="F47" s="40"/>
+      <c r="G47" s="41"/>
     </row>
     <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2341,7 +2338,7 @@
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="20">
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D4:G4"/>
     <mergeCell ref="B5:C5"/>
@@ -2351,6 +2348,7 @@
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="B21:E21"/>
     <mergeCell ref="B26:E26"/>

</xml_diff>

<commit_message>
Fix minor starting merit typo
</commit_message>
<xml_diff>
--- a/penyata-akhir-2023/form1/1AMANAH-2023.xlsx
+++ b/penyata-akhir-2023/form1/1AMANAH-2023.xlsx
@@ -445,7 +445,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
@@ -501,6 +501,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="bottom" wrapText="1" shrinkToFit="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="bottom" wrapText="1" shrinkToFit="1"/>
@@ -943,10 +946,10 @@
       </c>
       <c r="C14" s="20"/>
       <c r="D14" s="24">
-        <v>500</v>
-      </c>
-      <c r="E14" s="24"/>
-      <c r="F14" s="25">
+        <v>1000</v>
+      </c>
+      <c r="E14" s="25"/>
+      <c r="F14" s="26">
         <v>1000</v>
       </c>
       <c r="G14" s="6"/>
@@ -956,79 +959,79 @@
       <c r="B15" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="26"/>
+      <c r="C15" s="27"/>
       <c r="D15" s="23"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="24"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="25"/>
       <c r="G15" s="6"/>
     </row>
     <row r="16" ht="15.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="23"/>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="29">
+      <c r="D16" s="30">
         <v>2850</v>
       </c>
-      <c r="E16" s="30">
+      <c r="E16" s="31">
         <v>300</v>
       </c>
-      <c r="F16" s="24"/>
+      <c r="F16" s="25"/>
       <c r="G16" s="6"/>
     </row>
     <row r="17" ht="15.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="23"/>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="29">
+      <c r="D17" s="30">
         <v>3000</v>
       </c>
-      <c r="E17" s="24">
+      <c r="E17" s="25">
         <v>1700</v>
       </c>
-      <c r="F17" s="24"/>
+      <c r="F17" s="25"/>
       <c r="G17" s="6"/>
     </row>
     <row r="18" ht="15.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="23"/>
-      <c r="C18" s="28" t="s">
+      <c r="C18" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="29">
+      <c r="D18" s="30">
         <v>3085</v>
       </c>
-      <c r="E18" s="24">
+      <c r="E18" s="25">
         <v>1750</v>
       </c>
-      <c r="F18" s="24"/>
+      <c r="F18" s="25"/>
       <c r="G18" s="6"/>
     </row>
     <row r="19" ht="15.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="23"/>
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="29">
-        <v>0</v>
-      </c>
-      <c r="E19" s="24">
-        <v>0</v>
-      </c>
-      <c r="F19" s="24"/>
+      <c r="D19" s="30">
+        <v>0</v>
+      </c>
+      <c r="E19" s="25">
+        <v>0</v>
+      </c>
+      <c r="F19" s="25"/>
       <c r="G19" s="6"/>
     </row>
     <row r="20" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
-      <c r="B20" s="31"/>
+      <c r="B20" s="32"/>
       <c r="C20" s="16"/>
       <c r="D20" s="16"/>
       <c r="E20" s="17"/>
-      <c r="F20" s="32">
+      <c r="F20" s="33">
         <f>D16-E16+D17-E17+D18-E18+D19-E19+F14</f>
         <v>1000</v>
       </c>
@@ -1039,79 +1042,79 @@
       <c r="B21" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
       <c r="E21" s="20"/>
-      <c r="F21" s="24"/>
+      <c r="F21" s="25"/>
       <c r="G21" s="6"/>
     </row>
     <row r="22" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="23"/>
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="29">
-        <v>0</v>
-      </c>
-      <c r="E22" s="24">
-        <v>0</v>
-      </c>
-      <c r="F22" s="24"/>
+      <c r="D22" s="30">
+        <v>0</v>
+      </c>
+      <c r="E22" s="25">
+        <v>0</v>
+      </c>
+      <c r="F22" s="25"/>
       <c r="G22" s="6"/>
     </row>
     <row r="23" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="23"/>
-      <c r="C23" s="28" t="s">
+      <c r="C23" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="29">
-        <v>0</v>
-      </c>
-      <c r="E23" s="24">
-        <v>0</v>
-      </c>
-      <c r="F23" s="24"/>
+      <c r="D23" s="30">
+        <v>0</v>
+      </c>
+      <c r="E23" s="25">
+        <v>0</v>
+      </c>
+      <c r="F23" s="25"/>
       <c r="G23" s="6"/>
     </row>
     <row r="24" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="23"/>
-      <c r="C24" s="28" t="s">
+      <c r="C24" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="29">
-        <v>0</v>
-      </c>
-      <c r="E24" s="24">
+      <c r="D24" s="30">
+        <v>0</v>
+      </c>
+      <c r="E24" s="25">
         <v>200</v>
       </c>
-      <c r="F24" s="24"/>
+      <c r="F24" s="25"/>
       <c r="G24" s="6"/>
     </row>
     <row r="25" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="23"/>
-      <c r="C25" s="28" t="s">
+      <c r="C25" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="D25" s="29">
-        <v>0</v>
-      </c>
-      <c r="E25" s="24">
-        <v>0</v>
-      </c>
-      <c r="F25" s="24"/>
+      <c r="D25" s="30">
+        <v>0</v>
+      </c>
+      <c r="E25" s="25">
+        <v>0</v>
+      </c>
+      <c r="F25" s="25"/>
       <c r="G25" s="6"/>
     </row>
     <row r="26" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
-      <c r="B26" s="31"/>
+      <c r="B26" s="32"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
       <c r="E26" s="17"/>
-      <c r="F26" s="32">
+      <c r="F26" s="33">
         <f>D23-E23+D24-E24+D25-E25-E22+D22</f>
         <v>0</v>
       </c>
@@ -1122,71 +1125,71 @@
       <c r="B27" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
       <c r="E27" s="20"/>
-      <c r="F27" s="24"/>
+      <c r="F27" s="25"/>
       <c r="G27" s="6"/>
     </row>
     <row r="28" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="10"/>
-      <c r="C28" s="33" t="s">
+      <c r="C28" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="34"/>
-      <c r="E28" s="24">
-        <v>0</v>
-      </c>
-      <c r="F28" s="24"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="25">
+        <v>0</v>
+      </c>
+      <c r="F28" s="25"/>
       <c r="G28" s="6"/>
     </row>
     <row r="29" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="23"/>
-      <c r="C29" s="28" t="s">
+      <c r="C29" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="34"/>
-      <c r="E29" s="24">
+      <c r="D29" s="35"/>
+      <c r="E29" s="25">
         <v>1750</v>
       </c>
-      <c r="F29" s="24"/>
+      <c r="F29" s="25"/>
       <c r="G29" s="6"/>
     </row>
     <row r="30" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="23"/>
-      <c r="C30" s="28" t="s">
+      <c r="C30" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="34"/>
-      <c r="E30" s="24">
-        <v>0</v>
-      </c>
-      <c r="F30" s="24"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="25">
+        <v>0</v>
+      </c>
+      <c r="F30" s="25"/>
       <c r="G30" s="6"/>
     </row>
     <row r="31" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="23"/>
-      <c r="C31" s="28" t="s">
+      <c r="C31" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="D31" s="34"/>
-      <c r="E31" s="24">
-        <v>0</v>
-      </c>
-      <c r="F31" s="24"/>
+      <c r="D31" s="35"/>
+      <c r="E31" s="25">
+        <v>0</v>
+      </c>
+      <c r="F31" s="25"/>
       <c r="G31" s="6"/>
     </row>
     <row r="32" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
-      <c r="B32" s="31"/>
+      <c r="B32" s="32"/>
       <c r="C32" s="16"/>
       <c r="D32" s="16"/>
       <c r="E32" s="17"/>
-      <c r="F32" s="32">
+      <c r="F32" s="33">
         <f>-E28-E29-E30-E31</f>
         <v>0</v>
       </c>
@@ -1197,139 +1200,139 @@
       <c r="B33" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
       <c r="E33" s="20"/>
-      <c r="F33" s="24"/>
+      <c r="F33" s="25"/>
       <c r="G33" s="6"/>
     </row>
     <row r="34" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="23"/>
-      <c r="C34" s="35" t="s">
+      <c r="C34" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="29">
+      <c r="D34" s="30">
         <v>500</v>
       </c>
-      <c r="E34" s="24">
-        <v>0</v>
-      </c>
-      <c r="F34" s="24"/>
+      <c r="E34" s="25">
+        <v>0</v>
+      </c>
+      <c r="F34" s="25"/>
       <c r="G34" s="6"/>
     </row>
     <row r="35" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="23"/>
-      <c r="C35" s="35" t="s">
+      <c r="C35" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="D35" s="29">
+      <c r="D35" s="30">
         <v>100</v>
       </c>
-      <c r="E35" s="24">
-        <v>0</v>
-      </c>
-      <c r="F35" s="24"/>
+      <c r="E35" s="25">
+        <v>0</v>
+      </c>
+      <c r="F35" s="25"/>
       <c r="G35" s="6"/>
     </row>
     <row r="36" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="23"/>
-      <c r="C36" s="35" t="s">
+      <c r="C36" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="D36" s="29">
+      <c r="D36" s="30">
         <v>100</v>
       </c>
-      <c r="E36" s="24">
-        <v>0</v>
-      </c>
-      <c r="F36" s="24"/>
+      <c r="E36" s="25">
+        <v>0</v>
+      </c>
+      <c r="F36" s="25"/>
       <c r="G36" s="6"/>
     </row>
     <row r="37" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="23"/>
-      <c r="C37" s="35" t="s">
+      <c r="C37" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="D37" s="29">
-        <v>0</v>
-      </c>
-      <c r="E37" s="24">
-        <v>0</v>
-      </c>
-      <c r="F37" s="24"/>
+      <c r="D37" s="30">
+        <v>0</v>
+      </c>
+      <c r="E37" s="25">
+        <v>0</v>
+      </c>
+      <c r="F37" s="25"/>
       <c r="G37" s="6"/>
     </row>
     <row r="38" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="23"/>
-      <c r="C38" s="35" t="s">
+      <c r="C38" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="D38" s="29">
+      <c r="D38" s="30">
         <v>300</v>
       </c>
-      <c r="E38" s="24">
-        <v>0</v>
-      </c>
-      <c r="F38" s="24"/>
+      <c r="E38" s="25">
+        <v>0</v>
+      </c>
+      <c r="F38" s="25"/>
       <c r="G38" s="6"/>
     </row>
     <row r="39" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="23"/>
-      <c r="C39" s="35" t="s">
+      <c r="C39" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="D39" s="29">
+      <c r="D39" s="30">
         <v>100</v>
       </c>
-      <c r="E39" s="24">
-        <v>0</v>
-      </c>
-      <c r="F39" s="24"/>
+      <c r="E39" s="25">
+        <v>0</v>
+      </c>
+      <c r="F39" s="25"/>
       <c r="G39" s="6"/>
     </row>
     <row r="40" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="23"/>
-      <c r="C40" s="35" t="s">
+      <c r="C40" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="D40" s="35">
-        <v>0</v>
-      </c>
-      <c r="E40" s="27">
-        <v>0</v>
-      </c>
-      <c r="F40" s="24"/>
+      <c r="D40" s="36">
+        <v>0</v>
+      </c>
+      <c r="E40" s="28">
+        <v>0</v>
+      </c>
+      <c r="F40" s="25"/>
       <c r="G40" s="6"/>
     </row>
     <row r="41" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="23"/>
-      <c r="C41" s="35" t="s">
+      <c r="C41" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="D41" s="35">
-        <v>0</v>
-      </c>
-      <c r="E41" s="27">
-        <v>0</v>
-      </c>
-      <c r="F41" s="24"/>
+      <c r="D41" s="36">
+        <v>0</v>
+      </c>
+      <c r="E41" s="28">
+        <v>0</v>
+      </c>
+      <c r="F41" s="25"/>
       <c r="G41" s="6"/>
     </row>
     <row r="42" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
-      <c r="B42" s="31"/>
+      <c r="B42" s="32"/>
       <c r="C42" s="16"/>
       <c r="D42" s="16"/>
       <c r="E42" s="17"/>
-      <c r="F42" s="32">
+      <c r="F42" s="33">
         <f>D34-E34+D35-E35+D36-E36+D37-E37+D38-E38+D39-E39+D41-E41+D40-E40</f>
         <v>0</v>
       </c>
@@ -1337,13 +1340,13 @@
     </row>
     <row r="43" ht="15.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
-      <c r="B43" s="36" t="s">
+      <c r="B43" s="37" t="s">
         <v>29</v>
       </c>
       <c r="C43"/>
       <c r="D43"/>
       <c r="E43"/>
-      <c r="F43" s="37">
+      <c r="F43" s="38">
         <f>F20+F32+F26+F42</f>
         <v>1000</v>
       </c>
@@ -1355,7 +1358,7 @@
     </row>
     <row r="45" ht="18.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
-      <c r="B45" s="38" t="s">
+      <c r="B45" s="39" t="s">
         <v>30</v>
       </c>
       <c r="C45"/>
@@ -1366,7 +1369,7 @@
     </row>
     <row r="46" ht="18.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
-      <c r="B46" s="38" t="s">
+      <c r="B46" s="39" t="s">
         <v>31</v>
       </c>
       <c r="C46"/>
@@ -1376,13 +1379,13 @@
       <c r="G46" s="6"/>
     </row>
     <row r="47" ht="12.75" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="39"/>
-      <c r="B47" s="40"/>
-      <c r="C47" s="40"/>
-      <c r="D47" s="40"/>
-      <c r="E47" s="40"/>
-      <c r="F47" s="40"/>
-      <c r="G47" s="41"/>
+      <c r="A47" s="40"/>
+      <c r="B47" s="41"/>
+      <c r="C47" s="41"/>
+      <c r="D47" s="41"/>
+      <c r="E47" s="41"/>
+      <c r="F47" s="41"/>
+      <c r="G47" s="42"/>
     </row>
     <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>